<commit_message>
The project is ready to present
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demir\source\repos\oop\oop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC97F012-0DC4-406E-A2FA-BBD4B3FA3268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD0A5ED-B4C0-45F8-A0D8-3F3BC9F3765A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="888" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fruits" sheetId="1" r:id="rId1"/>
     <sheet name="Vegetables" sheetId="2" r:id="rId2"/>
-    <sheet name="Dairy" sheetId="3" r:id="rId3"/>
-    <sheet name="Meat" sheetId="4" r:id="rId4"/>
-    <sheet name="Dried" sheetId="5" r:id="rId5"/>
-    <sheet name="Snacks" sheetId="6" r:id="rId6"/>
+    <sheet name="Dairies and Cereal" sheetId="3" r:id="rId3"/>
+    <sheet name="Meat Products" sheetId="4" r:id="rId4"/>
+    <sheet name="Dried Fruits and Coffee" sheetId="5" r:id="rId5"/>
+    <sheet name="Snack Food" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -50,39 +50,21 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>90 kg</t>
-  </si>
-  <si>
     <t>Mandarin</t>
   </si>
   <si>
-    <t>100 kg</t>
-  </si>
-  <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>85 kg</t>
-  </si>
-  <si>
     <t>Banana</t>
   </si>
   <si>
-    <t>50 kg</t>
-  </si>
-  <si>
     <t>Strawberry</t>
   </si>
   <si>
-    <t xml:space="preserve">50 kg </t>
-  </si>
-  <si>
     <t>cucumber</t>
   </si>
   <si>
@@ -98,24 +80,12 @@
     <t>carrot</t>
   </si>
   <si>
-    <t xml:space="preserve">100 kg </t>
-  </si>
-  <si>
-    <t>80 kg</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
     <t>milk</t>
   </si>
   <si>
     <t>sek</t>
   </si>
   <si>
-    <t>pack</t>
-  </si>
-  <si>
     <t>cheese</t>
   </si>
   <si>
@@ -195,6 +165,21 @@
   </si>
   <si>
     <t>dido</t>
+  </si>
+  <si>
+    <t>bahceden</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>Packaged</t>
+  </si>
+  <si>
+    <t>Unpackaged</t>
+  </si>
+  <si>
+    <t>Cherry</t>
   </si>
 </sst>
 </file>
@@ -512,11 +497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="false">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,7 +511,7 @@
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -546,179 +531,124 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>321</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>1.2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="3">
-      <c r="A3">
-        <v>324</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3">
-        <v>2.3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
-      <c r="A4">
-        <v>323</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1.85</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
+      <c r="F4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>322</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>5.85</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="6">
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>325</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>9.85</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>kek</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>Ülker</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="inlineStr">
-        <is>
-          <t>unpacked</t>
-        </is>
-      </c>
-      <c r="E7" s="0">
-        <v>129</v>
-      </c>
-      <c r="F7" s="0" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D8" s="0" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E8" s="0">
-        <v>2</v>
-      </c>
-      <c r="F8" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D9" s="0" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E9" s="0">
-        <v>2</v>
-      </c>
-      <c r="F9" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="F6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -727,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +671,7 @@
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -761,129 +691,104 @@
         <v>3</v>
       </c>
     </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>421</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>5.23</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="3">
+      <c r="F2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>422</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>2.52</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>423</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1.25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
-      <c r="A5">
-        <v>424</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E5">
-        <v>2.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="6">
+        <v>5.3</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>425</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>6.25</v>
       </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D7" s="0" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E7" s="0">
-        <v>2</v>
-      </c>
-      <c r="F7" s="0" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="F6">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +801,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,16 +832,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>521</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>6.25</v>
@@ -947,56 +852,56 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>522</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>10.5</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
+      <c r="F3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>523</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>25.5</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
+      <c r="F4">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>524</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>5.25</v>
@@ -1007,16 +912,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>525</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>25.6</v>
@@ -1031,16 +936,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+    <sheetView workbookViewId="0" rightToLeft="false">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1060,18 +965,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
       <c r="A2">
-        <v>621</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>50.5</v>
@@ -1080,58 +985,58 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="3">
       <c r="A3">
-        <v>623</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3">
-        <v>40.299999999999997</v>
+        <v>40.3</v>
       </c>
       <c r="F3">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
       <c r="A4">
-        <v>622</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>60.5</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
       <c r="A5">
-        <v>624</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>20.3</v>
@@ -1140,24 +1045,50 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row spans="1:6" x14ac:dyDescent="0.3" outlineLevel="0" r="6">
       <c r="A6">
-        <v>625</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>15.5</v>
       </c>
       <c r="F6">
         <v>123</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Unpackaged</t>
+        </is>
+      </c>
+      <c r="E7" s="0">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1171,10 +1102,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1198,16 +1133,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>721</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>25.36</v>
@@ -1218,16 +1153,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>722</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>32.36</v>
@@ -1238,16 +1173,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>723</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>25.36</v>
@@ -1258,16 +1193,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>724</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>31.35</v>
@@ -1278,16 +1213,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>725</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>26.52</v>
@@ -1305,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,16 +1268,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>821</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>5.5</v>
@@ -1353,16 +1288,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>822</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>5.25</v>
@@ -1373,16 +1308,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>823</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>2.5</v>
@@ -1393,16 +1328,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>824</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>2.5</v>
@@ -1413,16 +1348,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>825</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>5.5</v>

</xml_diff>